<commit_message>
code for ugly comparison graph
</commit_message>
<xml_diff>
--- a/read_counts.xlsx
+++ b/read_counts.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vikas/Downloads/bootcamp/metagenomics/bmebootcamp-metagenomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A86BA6B-43CC-0041-9C9E-C2A738E2BFC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83043533-FA4D-B74A-826D-A648EAEE0A80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="read_counts" sheetId="1" r:id="rId1"/>
@@ -29,45 +29,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>bsubtilis_pb.ba</t>
-  </si>
-  <si>
-    <t>cneoformans_ont.ba</t>
-  </si>
-  <si>
-    <t>ecoli_pb.ba</t>
-  </si>
-  <si>
-    <t>efaecalis_pb.ba</t>
-  </si>
-  <si>
-    <t>k12_pb.ba</t>
-  </si>
-  <si>
-    <t>lfermentum_ontlumina.ba</t>
-  </si>
-  <si>
-    <t>lmonocytogenes_pb.ba</t>
-  </si>
-  <si>
-    <t>paeruginosa_pb.ba</t>
-  </si>
-  <si>
-    <t>saureus_pb.ba</t>
-  </si>
-  <si>
-    <t>scerevisiae_pb.ba</t>
-  </si>
-  <si>
-    <t>senterica_pb.ba</t>
-  </si>
-  <si>
     <t>file</t>
   </si>
   <si>
-    <t>reads aligned</t>
-  </si>
-  <si>
     <t xml:space="preserve">total reads in fastq (straight from fastq) </t>
   </si>
   <si>
@@ -78,12 +42,48 @@
   </si>
   <si>
     <t xml:space="preserve">note: this means there were a bunch of multimappers (reads that hit multiple references) </t>
+  </si>
+  <si>
+    <t>reads aligned (minimap2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads aligned (kraken2) </t>
+  </si>
+  <si>
+    <t>bsubtilis</t>
+  </si>
+  <si>
+    <t>cneoformans</t>
+  </si>
+  <si>
+    <t>ecoli</t>
+  </si>
+  <si>
+    <t>efaecalis</t>
+  </si>
+  <si>
+    <t>lfermentum</t>
+  </si>
+  <si>
+    <t>lmonocytogenes</t>
+  </si>
+  <si>
+    <t>paeruginosa</t>
+  </si>
+  <si>
+    <t>saureus</t>
+  </si>
+  <si>
+    <t>scerevisiae</t>
+  </si>
+  <si>
+    <t>senterica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -925,35 +925,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>901704</v>
@@ -962,10 +965,13 @@
         <f xml:space="preserve"> 100 * (B2 / A19)</f>
         <v>25.826504629961132</v>
       </c>
+      <c r="D2" s="1">
+        <v>636000</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>116935</v>
@@ -974,10 +980,13 @@
         <f xml:space="preserve"> 100 * (B3 / A19)</f>
         <v>3.3492391282555087</v>
       </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>531245</v>
@@ -986,10 +995,13 @@
         <f xml:space="preserve"> 100 * (B4 / A19)</f>
         <v>15.215859586010156</v>
       </c>
+      <c r="D4" s="1">
+        <v>187000</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>649559</v>
@@ -998,89 +1010,98 @@
         <f xml:space="preserve"> 100 * (B5 / A19)</f>
         <v>18.604595877286698</v>
       </c>
+      <c r="D5" s="1">
+        <v>392000</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>554073</v>
+        <v>777255</v>
       </c>
       <c r="C6" s="3">
         <f xml:space="preserve"> 100 * (B6 / A19)</f>
-        <v>15.869696596484495</v>
+        <v>22.262050358166803</v>
+      </c>
+      <c r="D6" s="1">
+        <v>514000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>777255</v>
+        <v>738425</v>
       </c>
       <c r="C7" s="3">
         <f xml:space="preserve"> 100 * (B7 / A19)</f>
-        <v>22.262050358166803</v>
+        <v>21.149885862077856</v>
+      </c>
+      <c r="D7" s="1">
+        <v>471000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>738425</v>
+        <v>344018</v>
       </c>
       <c r="C8" s="3">
         <f xml:space="preserve"> 100 * (B8 / A19)</f>
-        <v>21.149885862077856</v>
+        <v>9.8533248935237818</v>
+      </c>
+      <c r="D8" s="1">
+        <v>184000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>344018</v>
+        <v>702244</v>
       </c>
       <c r="C9" s="3">
         <f xml:space="preserve"> 100 * (B9 / A19)</f>
-        <v>9.8533248935237818</v>
+        <v>20.113593726280936</v>
+      </c>
+      <c r="D9" s="1">
+        <v>399000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>702244</v>
+        <v>107738</v>
       </c>
       <c r="C10" s="3">
         <f xml:space="preserve"> 100 * (B10 / A19)</f>
-        <v>20.113593726280936</v>
+        <v>3.0858196878607087</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>107738</v>
+        <v>532158</v>
       </c>
       <c r="C11" s="3">
         <f xml:space="preserve"> 100 * (B11 / A19)</f>
-        <v>3.0858196878607087</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>532158</v>
-      </c>
-      <c r="C12" s="3">
-        <f xml:space="preserve"> 100 * (B12 / A19)</f>
         <v>15.242009629402617</v>
+      </c>
+      <c r="D11" s="1">
+        <v>214000</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1088,7 +1109,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1098,16 +1119,16 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <f>SUM(B2:B12)</f>
-        <v>5955354</v>
+        <f>SUM(B2:B11)</f>
+        <v>5401281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>